<commit_message>
fix engine_node color, add engine_node route for xl_json_converter
</commit_message>
<xml_diff>
--- a/engine_node/xl_tools/tests/output_xl/nested.xlsx
+++ b/engine_node/xl_tools/tests/output_xl/nested.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>level_1</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>level_3</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3]</t>
   </si>
 </sst>
 </file>
@@ -383,27 +386,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:4">
       <c r="D1" s="1">
         <v>0</v>
       </c>
-      <c r="E1" s="1">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,7 +411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -425,17 +419,8 @@
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
+      <c r="D3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>